<commit_message>
Add template columns for ground wires, maintain optimize_phasing and target_fields, improve _plot_group_wires
</commit_message>
<xml_diff>
--- a/emf/templates/fields-template.xlsx
+++ b/emf/templates/fields-template.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
-  <si>
-    <t>FIELDS Template</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Frequency (Hertz)</t>
   </si>
@@ -104,6 +101,9 @@
   </si>
   <si>
     <t>Title</t>
+  </si>
+  <si>
+    <t>emf.fields template  - use emf.fields.load_template()</t>
   </si>
 </sst>
 </file>
@@ -420,7 +420,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -472,9 +472,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -523,6 +520,10 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -714,7 +715,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>template!$Q$7:$Q$8</c:f>
+              <c:f>template!$S$7:$S$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -729,7 +730,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>template!$P$5:$P$6</c:f>
+              <c:f>template!$R$5:$R$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -762,7 +763,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>template!$Q$5:$Q$6</c:f>
+              <c:f>template!$S$5:$S$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -777,7 +778,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>template!$P$5:$P$6</c:f>
+              <c:f>template!$R$5:$R$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -791,11 +792,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="68785280"/>
-        <c:axId val="68787200"/>
+        <c:axId val="121720192"/>
+        <c:axId val="82265984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="68785280"/>
+        <c:axId val="121720192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -820,12 +821,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68787200"/>
+        <c:crossAx val="82265984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68787200"/>
+        <c:axId val="82265984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -851,7 +852,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68785280"/>
+        <c:crossAx val="121720192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -864,7 +865,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1190,10 +1191,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="D8" sqref="D8:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1204,16 +1205,17 @@
     <col min="4" max="10" width="10.5703125" style="9" customWidth="1"/>
     <col min="11" max="11" width="10.5703125" style="14" customWidth="1"/>
     <col min="12" max="12" width="10.5703125" style="6" customWidth="1"/>
-    <col min="13" max="14" width="10.5703125" style="9" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" style="14" customWidth="1"/>
-    <col min="16" max="16" width="22.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="29"/>
+    <col min="13" max="15" width="10.5703125" style="9" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" style="9" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" style="14" customWidth="1"/>
+    <col min="18" max="18" width="22.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" style="28" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="27" customFormat="1" ht="15">
+    <row r="1" spans="1:19" s="26" customFormat="1" ht="15">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1228,9 +1230,11 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
-      <c r="O1" s="30"/>
-    </row>
-    <row r="2" spans="1:17" s="28" customFormat="1" ht="13.5" thickBot="1">
+      <c r="O1" s="1"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="29"/>
+    </row>
+    <row r="2" spans="1:19" s="27" customFormat="1" ht="13.5" thickBot="1">
       <c r="A2" s="3"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1245,122 +1249,132 @@
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
-      <c r="O2" s="33"/>
-    </row>
-    <row r="3" spans="1:17" ht="15.75">
-      <c r="A3" s="39" t="s">
+      <c r="O2" s="5"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="32"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75">
+      <c r="A3" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="39"/>
+      <c r="C3" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="S3" s="37"/>
+    </row>
+    <row r="4" spans="1:19" ht="38.25">
+      <c r="A4" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="35" t="s">
+      <c r="H4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="R4" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="S4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q3" s="38"/>
-    </row>
-    <row r="4" spans="1:17" ht="38.25">
-      <c r="A4" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="O4" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="P4" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q4" s="25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="17"/>
       <c r="L5" s="9"/>
-      <c r="P5" s="26">
+      <c r="R5" s="25">
         <f>MAX(E5:E25,N5:N26)*1.05</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="26">
+      <c r="S5" s="25">
         <f>B12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:19">
       <c r="A6" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="17"/>
       <c r="L6" s="9"/>
-      <c r="P6" s="26">
+      <c r="R6" s="25">
         <v>0</v>
       </c>
-      <c r="Q6" s="26">
+      <c r="S6" s="25">
         <f>B12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:19">
       <c r="A7" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="34">
+        <v>0</v>
+      </c>
+      <c r="B7" s="33">
         <v>60</v>
       </c>
       <c r="C7" s="12"/>
@@ -1373,36 +1387,36 @@
       <c r="J7" s="8"/>
       <c r="K7" s="15"/>
       <c r="L7" s="9"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26">
+      <c r="R7" s="25"/>
+      <c r="S7" s="25">
         <f>B13</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:19">
       <c r="A8" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="34">
+        <v>1</v>
+      </c>
+      <c r="B8" s="33">
         <v>100</v>
       </c>
       <c r="L8" s="9"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="26">
+      <c r="R8" s="25"/>
+      <c r="S8" s="25">
         <f>B13</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:19">
       <c r="A9" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="17"/>
       <c r="L9" s="9"/>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:19">
       <c r="A10" s="16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="12"/>
@@ -1416,25 +1430,25 @@
       <c r="K10" s="15"/>
       <c r="L10" s="9"/>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:19">
       <c r="A11" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="34">
+        <v>4</v>
+      </c>
+      <c r="B11" s="33">
         <v>3</v>
       </c>
       <c r="L11" s="9"/>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:19">
       <c r="A12" s="16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" s="17"/>
       <c r="L12" s="9"/>
     </row>
-    <row r="13" spans="1:17" ht="13.5" thickBot="1">
+    <row r="13" spans="1:19" ht="13.5" thickBot="1">
       <c r="A13" s="18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="19"/>
       <c r="C13" s="12"/>
@@ -1448,19 +1462,19 @@
       <c r="K13" s="15"/>
       <c r="L13" s="9"/>
     </row>
-    <row r="14" spans="1:17">
-      <c r="A14" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="42"/>
+    <row r="14" spans="1:19">
+      <c r="A14" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="41"/>
       <c r="L14" s="9"/>
     </row>
-    <row r="15" spans="1:17" ht="12.75" customHeight="1">
-      <c r="A15" s="43"/>
-      <c r="B15" s="44"/>
+    <row r="15" spans="1:19" ht="12.75" customHeight="1">
+      <c r="A15" s="42"/>
+      <c r="B15" s="43"/>
       <c r="L15" s="9"/>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:19">
       <c r="C16" s="12"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -1472,13 +1486,13 @@
       <c r="K16" s="15"/>
       <c r="L16" s="9"/>
     </row>
-    <row r="17" spans="3:14">
+    <row r="17" spans="3:15">
       <c r="L17" s="9"/>
     </row>
-    <row r="18" spans="3:14">
+    <row r="18" spans="3:15">
       <c r="L18" s="9"/>
     </row>
-    <row r="19" spans="3:14">
+    <row r="19" spans="3:15">
       <c r="C19" s="12"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -1490,14 +1504,16 @@
       <c r="K19" s="15"/>
       <c r="L19" s="9"/>
     </row>
-    <row r="20" spans="3:14">
+    <row r="20" spans="3:15">
       <c r="L20" s="9"/>
       <c r="N20"/>
-    </row>
-    <row r="21" spans="3:14">
+      <c r="O20"/>
+    </row>
+    <row r="21" spans="3:15">
       <c r="N21"/>
-    </row>
-    <row r="22" spans="3:14">
+      <c r="O21"/>
+    </row>
+    <row r="22" spans="3:15">
       <c r="C22" s="12"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -1508,14 +1524,17 @@
       <c r="J22" s="8"/>
       <c r="K22" s="15"/>
       <c r="N22"/>
-    </row>
-    <row r="23" spans="3:14">
+      <c r="O22"/>
+    </row>
+    <row r="23" spans="3:15">
       <c r="N23"/>
-    </row>
-    <row r="24" spans="3:14">
+      <c r="O23"/>
+    </row>
+    <row r="24" spans="3:15">
       <c r="N24"/>
-    </row>
-    <row r="25" spans="3:14">
+      <c r="O24"/>
+    </row>
+    <row r="25" spans="3:15">
       <c r="C25" s="12"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
@@ -1526,25 +1545,27 @@
       <c r="J25" s="8"/>
       <c r="K25" s="15"/>
       <c r="N25"/>
-    </row>
-    <row r="26" spans="3:14">
-      <c r="C26" s="32"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="31"/>
+      <c r="O25"/>
+    </row>
+    <row r="26" spans="3:15">
+      <c r="C26" s="31"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
       <c r="L26" s="11"/>
       <c r="N26"/>
+      <c r="O26"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C3:K3"/>
-    <mergeCell ref="L3:O3"/>
-    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="L3:Q3"/>
+    <mergeCell ref="R3:S3"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A14:B15"/>
   </mergeCells>

</xml_diff>

<commit_message>
various small updates, mostly docs
</commit_message>
<xml_diff>
--- a/emf/templates/fields-template.xlsx
+++ b/emf/templates/fields-template.xlsx
@@ -40,9 +40,6 @@
     <t>Subconductors per Bundle</t>
   </si>
   <si>
-    <t>Phase-Phase (kV)</t>
-  </si>
-  <si>
     <t>Phase Current (Amp)</t>
   </si>
   <si>
@@ -104,6 +101,9 @@
   </si>
   <si>
     <t>emf.fields template  - use emf.fields.load_template()</t>
+  </si>
+  <si>
+    <t>Phase-Phase Voltage (kV)</t>
   </si>
 </sst>
 </file>
@@ -491,39 +491,39 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -792,11 +792,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="121720192"/>
-        <c:axId val="82265984"/>
+        <c:axId val="129076224"/>
+        <c:axId val="74729344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121720192"/>
+        <c:axId val="129076224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -821,12 +821,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82265984"/>
+        <c:crossAx val="74729344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82265984"/>
+        <c:axId val="74729344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -852,7 +852,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121720192"/>
+        <c:crossAx val="129076224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -865,7 +865,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1194,7 +1194,7 @@
   <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D9"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1215,7 +1215,7 @@
   <sheetData>
     <row r="1" spans="1:19" s="26" customFormat="1" ht="15">
       <c r="A1" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1231,7 +1231,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
-      <c r="P1" s="44"/>
+      <c r="P1" s="34"/>
       <c r="Q1" s="29"/>
     </row>
     <row r="2" spans="1:19" s="27" customFormat="1" ht="13.5" thickBot="1">
@@ -1250,100 +1250,100 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
-      <c r="P2" s="45"/>
+      <c r="P2" s="35"/>
       <c r="Q2" s="32"/>
     </row>
     <row r="3" spans="1:19" ht="15.75">
-      <c r="A3" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="34" t="s">
+      <c r="A3" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="41"/>
+      <c r="C3" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="S3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="S3" s="39"/>
     </row>
     <row r="4" spans="1:19" ht="38.25">
       <c r="A4" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="23" t="s">
-        <v>23</v>
-      </c>
       <c r="C4" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>20</v>
-      </c>
       <c r="I4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="K4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="L4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" s="10" t="s">
+      <c r="O4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="P4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="Q4" s="13" t="s">
-        <v>10</v>
-      </c>
       <c r="R4" s="24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S4" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="17"/>
       <c r="L5" s="9"/>
@@ -1358,7 +1358,7 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="17"/>
       <c r="L6" s="9"/>
@@ -1409,7 +1409,7 @@
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="17"/>
       <c r="L9" s="9"/>
@@ -1463,15 +1463,15 @@
       <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="41"/>
+      <c r="A14" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="43"/>
       <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:19" ht="12.75" customHeight="1">
-      <c r="A15" s="42"/>
-      <c r="B15" s="43"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="45"/>
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:19">

</xml_diff>